<commit_message>
Casos de prueba nuevos
</commit_message>
<xml_diff>
--- a/Documentacion/3-Archivos de prueba/Casos de prueba Ayed 2021.xlsx
+++ b/Documentacion/3-Archivos de prueba/Casos de prueba Ayed 2021.xlsx
@@ -12,15 +12,15 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="134" uniqueCount="82">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="158" uniqueCount="101">
   <si>
     <t>Plantilla de Casos de Pruebas de Software</t>
   </si>
   <si>
-    <t>Proyecto: [Nombre del Proyecto]</t>
+    <t>Proyecto: Algoritmos y estructuras de datos 2021</t>
   </si>
   <si>
-    <t>Ciclo de Pruebas: [Descripción del Ciclo de Pruebas]</t>
+    <t>Ciclo de Pruebas: smoke test</t>
   </si>
   <si>
     <t>Información para el Seguimiento</t>
@@ -203,6 +203,63 @@
     <t>ver si se puede evitar que el programa deje de funcionar.</t>
   </si>
   <si>
+    <t>Campo vacio en elecion_test.txt</t>
+  </si>
+  <si>
+    <t>Se deja un campo id_vino vacio</t>
+  </si>
+  <si>
+    <t>Iniciar el programa</t>
+  </si>
+  <si>
+    <t>Cargar datos a la lista de membresias</t>
+  </si>
+  <si>
+    <t>43576   -	02  -	2021    -	62534    -   15645    -   23467    -       -	23467    -   97453 ;</t>
+  </si>
+  <si>
+    <t xml:space="preserve">El programa carga la lista </t>
+  </si>
+  <si>
+    <t>Se produce un error al iniciar el programa</t>
+  </si>
+  <si>
+    <t>Campo 0 en elecion_test.txt</t>
+  </si>
+  <si>
+    <t>Se inserta un 0 en un campo cualquiera</t>
+  </si>
+  <si>
+    <t>Rankings</t>
+  </si>
+  <si>
+    <t>Correr ranking de vinos o de bodegas</t>
+  </si>
+  <si>
+    <t>74534   -	04  -	0    -	74457    -   74563    -   45646    -   81633    - 	62534    -   15645 ;</t>
+  </si>
+  <si>
+    <t>Los rankings se muestren</t>
+  </si>
+  <si>
+    <t>La aplicación maneja correctamente el caso</t>
+  </si>
+  <si>
+    <t>Ok</t>
+  </si>
+  <si>
+    <t>Edad Usuario con letras</t>
+  </si>
+  <si>
+    <t>Se inserta una letra en el campo edad</t>
+  </si>
+  <si>
+    <t>72953   -       Mario Martinez      -    Mercedes 283, El Chalten, Río Negro     -     0AA  ;</t>
+  </si>
+  <si>
+    <t>El usuario es cargado con la edad en 0</t>
+  </si>
+  <si>
     <t>Descripción de la información a completar en cada columna</t>
   </si>
   <si>
@@ -372,7 +429,7 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="15">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
@@ -384,6 +441,9 @@
     </xf>
     <xf borderId="1" fillId="2" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment shrinkToFit="0" vertical="bottom" wrapText="0"/>
+    </xf>
+    <xf borderId="1" fillId="2" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
     <xf borderId="2" fillId="3" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1">
       <alignment horizontal="center" shrinkToFit="0" vertical="center" wrapText="1"/>
@@ -635,16 +695,16 @@
   <cols>
     <col customWidth="1" min="1" max="1" width="7.86"/>
     <col customWidth="1" min="2" max="2" width="25.0"/>
-    <col customWidth="1" min="3" max="3" width="61.43"/>
+    <col customWidth="1" min="3" max="3" width="81.57"/>
     <col customWidth="1" min="4" max="4" width="13.71"/>
     <col customWidth="1" min="5" max="5" width="25.86"/>
     <col customWidth="1" min="6" max="6" width="19.71"/>
-    <col customWidth="1" min="7" max="7" width="27.57"/>
-    <col customWidth="1" min="8" max="8" width="32.57"/>
-    <col customWidth="1" min="9" max="9" width="31.71"/>
+    <col customWidth="1" min="7" max="7" width="30.71"/>
+    <col customWidth="1" min="8" max="8" width="45.29"/>
+    <col customWidth="1" min="9" max="9" width="24.86"/>
     <col customWidth="1" min="10" max="10" width="31.86"/>
-    <col customWidth="1" min="11" max="11" width="26.71"/>
-    <col customWidth="1" min="12" max="12" width="30.29"/>
+    <col customWidth="1" min="11" max="11" width="20.57"/>
+    <col customWidth="1" min="12" max="12" width="56.14"/>
     <col customWidth="1" min="13" max="13" width="10.71"/>
     <col customWidth="1" min="14" max="14" width="21.71"/>
     <col customWidth="1" min="15" max="15" width="32.43"/>
@@ -710,7 +770,7 @@
       <c r="Z2" s="2"/>
     </row>
     <row r="3">
-      <c r="A3" s="2" t="s">
+      <c r="A3" s="4" t="s">
         <v>1</v>
       </c>
       <c r="B3" s="2"/>
@@ -740,10 +800,10 @@
       <c r="Z3" s="2"/>
     </row>
     <row r="4">
-      <c r="A4" s="2" t="s">
+      <c r="A4" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="B4" s="2"/>
+      <c r="B4" s="4"/>
       <c r="C4" s="2"/>
       <c r="D4" s="2"/>
       <c r="E4" s="2"/>
@@ -781,7 +841,7 @@
       <c r="I5" s="2"/>
       <c r="J5" s="2"/>
       <c r="K5" s="2"/>
-      <c r="L5" s="4" t="s">
+      <c r="L5" s="5" t="s">
         <v>3</v>
       </c>
       <c r="M5" s="2"/>
@@ -800,49 +860,49 @@
       <c r="Z5" s="2"/>
     </row>
     <row r="6" ht="30.0" customHeight="1">
-      <c r="A6" s="5" t="s">
+      <c r="A6" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="B6" s="5" t="s">
+      <c r="B6" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="C6" s="5" t="s">
+      <c r="C6" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="D6" s="5" t="s">
+      <c r="D6" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="E6" s="5" t="s">
+      <c r="E6" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="F6" s="5" t="s">
+      <c r="F6" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="G6" s="5" t="s">
+      <c r="G6" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="H6" s="5" t="s">
+      <c r="H6" s="6" t="s">
         <v>11</v>
       </c>
-      <c r="I6" s="5" t="s">
+      <c r="I6" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="J6" s="5" t="s">
+      <c r="J6" s="6" t="s">
         <v>13</v>
       </c>
-      <c r="K6" s="5" t="s">
+      <c r="K6" s="6" t="s">
         <v>14</v>
       </c>
-      <c r="L6" s="4" t="s">
+      <c r="L6" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="M6" s="4" t="s">
+      <c r="M6" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="N6" s="4" t="s">
+      <c r="N6" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="O6" s="4" t="s">
+      <c r="O6" s="5" t="s">
         <v>18</v>
       </c>
       <c r="P6" s="2"/>
@@ -858,49 +918,49 @@
       <c r="Z6" s="2"/>
     </row>
     <row r="7">
-      <c r="A7" s="6">
+      <c r="A7" s="7">
         <v>1.0</v>
       </c>
-      <c r="B7" s="6" t="s">
+      <c r="B7" s="7" t="s">
         <v>19</v>
       </c>
-      <c r="C7" s="6" t="s">
+      <c r="C7" s="7" t="s">
         <v>20</v>
       </c>
-      <c r="D7" s="7">
+      <c r="D7" s="8">
         <v>44499.0</v>
       </c>
-      <c r="E7" s="6" t="s">
+      <c r="E7" s="7" t="s">
         <v>21</v>
       </c>
-      <c r="F7" s="6" t="s">
+      <c r="F7" s="7" t="s">
         <v>22</v>
       </c>
-      <c r="G7" s="6" t="s">
+      <c r="G7" s="7" t="s">
         <v>23</v>
       </c>
-      <c r="H7" s="6" t="s">
+      <c r="H7" s="7" t="s">
         <v>24</v>
       </c>
-      <c r="I7" s="6" t="s">
+      <c r="I7" s="7" t="s">
         <v>25</v>
       </c>
-      <c r="J7" s="6" t="s">
+      <c r="J7" s="7" t="s">
         <v>25</v>
       </c>
-      <c r="K7" s="6" t="s">
+      <c r="K7" s="7" t="s">
         <v>25</v>
       </c>
-      <c r="L7" s="6" t="s">
+      <c r="L7" s="7" t="s">
         <v>26</v>
       </c>
-      <c r="M7" s="6" t="s">
+      <c r="M7" s="7" t="s">
         <v>27</v>
       </c>
-      <c r="N7" s="7">
+      <c r="N7" s="8">
         <v>44499.0</v>
       </c>
-      <c r="O7" s="6" t="s">
+      <c r="O7" s="7" t="s">
         <v>25</v>
       </c>
       <c r="P7" s="2"/>
@@ -916,49 +976,49 @@
       <c r="Z7" s="2"/>
     </row>
     <row r="8">
-      <c r="A8" s="6">
+      <c r="A8" s="7">
         <v>2.0</v>
       </c>
-      <c r="B8" s="6" t="s">
+      <c r="B8" s="7" t="s">
         <v>28</v>
       </c>
-      <c r="C8" s="6" t="s">
+      <c r="C8" s="7" t="s">
         <v>20</v>
       </c>
-      <c r="D8" s="7">
+      <c r="D8" s="8">
         <v>44499.0</v>
       </c>
-      <c r="E8" s="6" t="s">
+      <c r="E8" s="7" t="s">
         <v>21</v>
       </c>
-      <c r="F8" s="6" t="s">
+      <c r="F8" s="7" t="s">
         <v>22</v>
       </c>
-      <c r="G8" s="6" t="s">
+      <c r="G8" s="7" t="s">
         <v>29</v>
       </c>
-      <c r="H8" s="6" t="s">
+      <c r="H8" s="7" t="s">
         <v>24</v>
       </c>
-      <c r="I8" s="6" t="s">
+      <c r="I8" s="7" t="s">
         <v>25</v>
       </c>
-      <c r="J8" s="6" t="s">
+      <c r="J8" s="7" t="s">
         <v>25</v>
       </c>
-      <c r="K8" s="6" t="s">
+      <c r="K8" s="7" t="s">
         <v>25</v>
       </c>
-      <c r="L8" s="6" t="s">
+      <c r="L8" s="7" t="s">
         <v>26</v>
       </c>
-      <c r="M8" s="6" t="s">
+      <c r="M8" s="7" t="s">
         <v>27</v>
       </c>
-      <c r="N8" s="7">
+      <c r="N8" s="8">
         <v>44499.0</v>
       </c>
-      <c r="O8" s="6" t="s">
+      <c r="O8" s="7" t="s">
         <v>25</v>
       </c>
       <c r="P8" s="2"/>
@@ -974,49 +1034,49 @@
       <c r="Z8" s="2"/>
     </row>
     <row r="9">
-      <c r="A9" s="6">
+      <c r="A9" s="7">
         <v>3.0</v>
       </c>
-      <c r="B9" s="6" t="s">
+      <c r="B9" s="7" t="s">
         <v>30</v>
       </c>
-      <c r="C9" s="6" t="s">
+      <c r="C9" s="7" t="s">
         <v>31</v>
       </c>
-      <c r="D9" s="7">
+      <c r="D9" s="8">
         <v>44499.0</v>
       </c>
-      <c r="E9" s="6" t="s">
+      <c r="E9" s="7" t="s">
         <v>21</v>
       </c>
-      <c r="F9" s="6" t="s">
+      <c r="F9" s="7" t="s">
         <v>22</v>
       </c>
-      <c r="G9" s="6" t="s">
+      <c r="G9" s="7" t="s">
         <v>32</v>
       </c>
-      <c r="H9" s="6" t="s">
+      <c r="H9" s="7" t="s">
         <v>24</v>
       </c>
-      <c r="I9" s="6" t="s">
+      <c r="I9" s="7" t="s">
         <v>25</v>
       </c>
-      <c r="J9" s="6" t="s">
+      <c r="J9" s="7" t="s">
         <v>25</v>
       </c>
-      <c r="K9" s="6" t="s">
+      <c r="K9" s="7" t="s">
         <v>25</v>
       </c>
-      <c r="L9" s="6" t="s">
+      <c r="L9" s="7" t="s">
         <v>33</v>
       </c>
-      <c r="M9" s="6" t="s">
+      <c r="M9" s="7" t="s">
         <v>34</v>
       </c>
-      <c r="N9" s="7">
+      <c r="N9" s="8">
         <v>44499.0</v>
       </c>
-      <c r="O9" s="6" t="s">
+      <c r="O9" s="7" t="s">
         <v>25</v>
       </c>
       <c r="P9" s="2"/>
@@ -1032,49 +1092,49 @@
       <c r="Z9" s="2"/>
     </row>
     <row r="10">
-      <c r="A10" s="6">
+      <c r="A10" s="7">
         <v>4.0</v>
       </c>
-      <c r="B10" s="6" t="s">
+      <c r="B10" s="7" t="s">
         <v>35</v>
       </c>
-      <c r="C10" s="6" t="s">
+      <c r="C10" s="7" t="s">
         <v>36</v>
       </c>
-      <c r="D10" s="7">
+      <c r="D10" s="8">
         <v>44499.0</v>
       </c>
-      <c r="E10" s="6" t="s">
+      <c r="E10" s="7" t="s">
         <v>21</v>
       </c>
-      <c r="F10" s="6" t="s">
+      <c r="F10" s="7" t="s">
         <v>22</v>
       </c>
-      <c r="G10" s="6" t="s">
+      <c r="G10" s="7" t="s">
         <v>37</v>
       </c>
-      <c r="H10" s="6" t="s">
+      <c r="H10" s="7" t="s">
         <v>24</v>
       </c>
-      <c r="I10" s="6" t="s">
+      <c r="I10" s="7" t="s">
         <v>25</v>
       </c>
-      <c r="J10" s="6" t="s">
+      <c r="J10" s="7" t="s">
         <v>25</v>
       </c>
-      <c r="K10" s="6" t="s">
+      <c r="K10" s="7" t="s">
         <v>25</v>
       </c>
-      <c r="L10" s="6" t="s">
+      <c r="L10" s="7" t="s">
         <v>38</v>
       </c>
-      <c r="M10" s="6" t="s">
+      <c r="M10" s="7" t="s">
         <v>39</v>
       </c>
-      <c r="N10" s="7">
+      <c r="N10" s="8">
         <v>44499.0</v>
       </c>
-      <c r="O10" s="6" t="s">
+      <c r="O10" s="7" t="s">
         <v>25</v>
       </c>
       <c r="P10" s="2"/>
@@ -1090,49 +1150,49 @@
       <c r="Z10" s="2"/>
     </row>
     <row r="11">
-      <c r="A11" s="6">
+      <c r="A11" s="7">
         <v>5.0</v>
       </c>
-      <c r="B11" s="6" t="s">
+      <c r="B11" s="7" t="s">
         <v>40</v>
       </c>
-      <c r="C11" s="6" t="s">
+      <c r="C11" s="7" t="s">
         <v>41</v>
       </c>
-      <c r="D11" s="7">
+      <c r="D11" s="8">
         <v>44499.0</v>
       </c>
-      <c r="E11" s="6" t="s">
+      <c r="E11" s="7" t="s">
         <v>21</v>
       </c>
-      <c r="F11" s="6" t="s">
+      <c r="F11" s="7" t="s">
         <v>42</v>
       </c>
-      <c r="G11" s="6" t="s">
+      <c r="G11" s="7" t="s">
         <v>43</v>
       </c>
-      <c r="H11" s="6" t="s">
+      <c r="H11" s="7" t="s">
         <v>44</v>
       </c>
-      <c r="I11" s="6" t="s">
+      <c r="I11" s="7" t="s">
         <v>25</v>
       </c>
-      <c r="J11" s="6" t="s">
+      <c r="J11" s="7" t="s">
         <v>25</v>
       </c>
-      <c r="K11" s="6" t="s">
+      <c r="K11" s="7" t="s">
         <v>25</v>
       </c>
-      <c r="L11" s="6" t="s">
+      <c r="L11" s="7" t="s">
         <v>45</v>
       </c>
-      <c r="M11" s="6" t="s">
+      <c r="M11" s="7" t="s">
         <v>27</v>
       </c>
-      <c r="N11" s="7">
+      <c r="N11" s="8">
         <v>44499.0</v>
       </c>
-      <c r="O11" s="6" t="s">
+      <c r="O11" s="7" t="s">
         <v>25</v>
       </c>
       <c r="P11" s="2"/>
@@ -1148,49 +1208,49 @@
       <c r="Z11" s="2"/>
     </row>
     <row r="12">
-      <c r="A12" s="6">
+      <c r="A12" s="7">
         <v>6.0</v>
       </c>
-      <c r="B12" s="6" t="s">
+      <c r="B12" s="7" t="s">
         <v>46</v>
       </c>
-      <c r="C12" s="6" t="s">
+      <c r="C12" s="7" t="s">
         <v>47</v>
       </c>
-      <c r="D12" s="7">
+      <c r="D12" s="8">
         <v>44499.0</v>
       </c>
-      <c r="E12" s="6" t="s">
+      <c r="E12" s="7" t="s">
         <v>48</v>
       </c>
-      <c r="F12" s="6" t="s">
+      <c r="F12" s="7" t="s">
         <v>49</v>
       </c>
-      <c r="G12" s="6" t="s">
+      <c r="G12" s="7" t="s">
         <v>50</v>
       </c>
-      <c r="H12" s="6" t="s">
+      <c r="H12" s="7" t="s">
         <v>51</v>
       </c>
-      <c r="I12" s="6" t="s">
+      <c r="I12" s="7" t="s">
         <v>25</v>
       </c>
-      <c r="J12" s="6" t="s">
+      <c r="J12" s="7" t="s">
         <v>25</v>
       </c>
-      <c r="K12" s="6" t="s">
+      <c r="K12" s="7" t="s">
         <v>25</v>
       </c>
-      <c r="L12" s="6" t="s">
+      <c r="L12" s="7" t="s">
         <v>52</v>
       </c>
-      <c r="M12" s="6" t="s">
+      <c r="M12" s="7" t="s">
         <v>39</v>
       </c>
-      <c r="N12" s="7">
+      <c r="N12" s="8">
         <v>44499.0</v>
       </c>
-      <c r="O12" s="6" t="s">
+      <c r="O12" s="7" t="s">
         <v>53</v>
       </c>
       <c r="P12" s="2"/>
@@ -1206,49 +1266,49 @@
       <c r="Z12" s="2"/>
     </row>
     <row r="13">
-      <c r="A13" s="6">
+      <c r="A13" s="7">
         <v>7.0</v>
       </c>
-      <c r="B13" s="6" t="s">
+      <c r="B13" s="7" t="s">
         <v>54</v>
       </c>
-      <c r="C13" s="6" t="s">
+      <c r="C13" s="7" t="s">
         <v>55</v>
       </c>
-      <c r="D13" s="7">
+      <c r="D13" s="8">
         <v>44501.0</v>
       </c>
-      <c r="E13" s="6" t="s">
+      <c r="E13" s="7" t="s">
         <v>21</v>
       </c>
-      <c r="F13" s="6" t="s">
+      <c r="F13" s="7" t="s">
         <v>42</v>
       </c>
-      <c r="G13" s="6" t="s">
+      <c r="G13" s="7" t="s">
         <v>56</v>
       </c>
-      <c r="H13" s="6" t="s">
+      <c r="H13" s="7" t="s">
         <v>44</v>
       </c>
-      <c r="I13" s="6" t="s">
+      <c r="I13" s="7" t="s">
         <v>25</v>
       </c>
-      <c r="J13" s="6" t="s">
+      <c r="J13" s="7" t="s">
         <v>25</v>
       </c>
-      <c r="K13" s="6" t="s">
+      <c r="K13" s="7" t="s">
         <v>25</v>
       </c>
-      <c r="L13" s="6" t="s">
+      <c r="L13" s="7" t="s">
         <v>45</v>
       </c>
-      <c r="M13" s="6" t="s">
+      <c r="M13" s="7" t="s">
         <v>27</v>
       </c>
-      <c r="N13" s="7">
+      <c r="N13" s="8">
         <v>44501.0</v>
       </c>
-      <c r="O13" s="6" t="s">
+      <c r="O13" s="7" t="s">
         <v>25</v>
       </c>
       <c r="P13" s="2"/>
@@ -1264,49 +1324,49 @@
       <c r="Z13" s="2"/>
     </row>
     <row r="14">
-      <c r="A14" s="6">
+      <c r="A14" s="7">
         <v>8.0</v>
       </c>
-      <c r="B14" s="6" t="s">
+      <c r="B14" s="7" t="s">
         <v>57</v>
       </c>
-      <c r="C14" s="6" t="s">
+      <c r="C14" s="7" t="s">
         <v>58</v>
       </c>
-      <c r="D14" s="7">
+      <c r="D14" s="8">
         <v>44501.0</v>
       </c>
-      <c r="E14" s="6" t="s">
+      <c r="E14" s="7" t="s">
         <v>48</v>
       </c>
-      <c r="F14" s="6" t="s">
+      <c r="F14" s="7" t="s">
         <v>59</v>
       </c>
-      <c r="G14" s="6" t="s">
+      <c r="G14" s="7" t="s">
         <v>60</v>
       </c>
-      <c r="H14" s="6" t="s">
+      <c r="H14" s="7" t="s">
         <v>51</v>
       </c>
-      <c r="I14" s="6" t="s">
+      <c r="I14" s="7" t="s">
         <v>25</v>
       </c>
-      <c r="J14" s="6" t="s">
+      <c r="J14" s="7" t="s">
         <v>25</v>
       </c>
-      <c r="K14" s="6" t="s">
+      <c r="K14" s="7" t="s">
         <v>25</v>
       </c>
-      <c r="L14" s="6" t="s">
+      <c r="L14" s="7" t="s">
         <v>61</v>
       </c>
-      <c r="M14" s="6" t="s">
+      <c r="M14" s="7" t="s">
         <v>39</v>
       </c>
-      <c r="N14" s="7">
+      <c r="N14" s="8">
         <v>44501.0</v>
       </c>
-      <c r="O14" s="6" t="s">
+      <c r="O14" s="7" t="s">
         <v>62</v>
       </c>
       <c r="P14" s="2"/>
@@ -1322,21 +1382,41 @@
       <c r="Z14" s="2"/>
     </row>
     <row r="15">
-      <c r="A15" s="8"/>
-      <c r="B15" s="8"/>
-      <c r="C15" s="8"/>
-      <c r="D15" s="8"/>
-      <c r="E15" s="8"/>
-      <c r="F15" s="8"/>
-      <c r="G15" s="8"/>
-      <c r="H15" s="8"/>
-      <c r="I15" s="8"/>
-      <c r="J15" s="8"/>
-      <c r="K15" s="8"/>
-      <c r="L15" s="8"/>
-      <c r="M15" s="8"/>
-      <c r="N15" s="8"/>
-      <c r="O15" s="8"/>
+      <c r="A15" s="7">
+        <v>9.0</v>
+      </c>
+      <c r="B15" s="7" t="s">
+        <v>63</v>
+      </c>
+      <c r="C15" s="7" t="s">
+        <v>64</v>
+      </c>
+      <c r="D15" s="8">
+        <v>44505.0</v>
+      </c>
+      <c r="E15" s="7" t="s">
+        <v>65</v>
+      </c>
+      <c r="F15" s="7" t="s">
+        <v>66</v>
+      </c>
+      <c r="G15" s="7" t="s">
+        <v>67</v>
+      </c>
+      <c r="H15" s="7" t="s">
+        <v>68</v>
+      </c>
+      <c r="I15" s="9"/>
+      <c r="J15" s="9"/>
+      <c r="K15" s="9"/>
+      <c r="L15" s="7" t="s">
+        <v>69</v>
+      </c>
+      <c r="M15" s="7" t="s">
+        <v>39</v>
+      </c>
+      <c r="N15" s="9"/>
+      <c r="O15" s="9"/>
       <c r="P15" s="2"/>
       <c r="Q15" s="2"/>
       <c r="R15" s="2"/>
@@ -1350,21 +1430,41 @@
       <c r="Z15" s="2"/>
     </row>
     <row r="16">
-      <c r="A16" s="8"/>
-      <c r="B16" s="8"/>
-      <c r="C16" s="8"/>
-      <c r="D16" s="8"/>
-      <c r="E16" s="8"/>
-      <c r="F16" s="8"/>
-      <c r="G16" s="8"/>
-      <c r="H16" s="8"/>
-      <c r="I16" s="8"/>
-      <c r="J16" s="8"/>
-      <c r="K16" s="8"/>
-      <c r="L16" s="8"/>
-      <c r="M16" s="8"/>
-      <c r="N16" s="8"/>
-      <c r="O16" s="8"/>
+      <c r="A16" s="7">
+        <v>10.0</v>
+      </c>
+      <c r="B16" s="7" t="s">
+        <v>70</v>
+      </c>
+      <c r="C16" s="7" t="s">
+        <v>71</v>
+      </c>
+      <c r="D16" s="8">
+        <v>44505.0</v>
+      </c>
+      <c r="E16" s="7" t="s">
+        <v>72</v>
+      </c>
+      <c r="F16" s="7" t="s">
+        <v>73</v>
+      </c>
+      <c r="G16" s="7" t="s">
+        <v>74</v>
+      </c>
+      <c r="H16" s="7" t="s">
+        <v>75</v>
+      </c>
+      <c r="I16" s="9"/>
+      <c r="J16" s="9"/>
+      <c r="K16" s="9"/>
+      <c r="L16" s="7" t="s">
+        <v>76</v>
+      </c>
+      <c r="M16" s="7" t="s">
+        <v>77</v>
+      </c>
+      <c r="N16" s="9"/>
+      <c r="O16" s="7"/>
       <c r="P16" s="2"/>
       <c r="Q16" s="2"/>
       <c r="R16" s="2"/>
@@ -1378,21 +1478,41 @@
       <c r="Z16" s="2"/>
     </row>
     <row r="17">
-      <c r="A17" s="8"/>
-      <c r="B17" s="8"/>
-      <c r="C17" s="8"/>
-      <c r="D17" s="8"/>
-      <c r="E17" s="8"/>
-      <c r="F17" s="8"/>
-      <c r="G17" s="8"/>
-      <c r="H17" s="8"/>
-      <c r="I17" s="8"/>
-      <c r="J17" s="8"/>
-      <c r="K17" s="8"/>
-      <c r="L17" s="8"/>
-      <c r="M17" s="8"/>
-      <c r="N17" s="8"/>
-      <c r="O17" s="8"/>
+      <c r="A17" s="7">
+        <v>11.0</v>
+      </c>
+      <c r="B17" s="7" t="s">
+        <v>78</v>
+      </c>
+      <c r="C17" s="7" t="s">
+        <v>79</v>
+      </c>
+      <c r="D17" s="8">
+        <v>44505.0</v>
+      </c>
+      <c r="E17" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="F17" s="7" t="s">
+        <v>22</v>
+      </c>
+      <c r="G17" s="7" t="s">
+        <v>80</v>
+      </c>
+      <c r="H17" s="7" t="s">
+        <v>24</v>
+      </c>
+      <c r="I17" s="9"/>
+      <c r="J17" s="9"/>
+      <c r="K17" s="9"/>
+      <c r="L17" s="7" t="s">
+        <v>81</v>
+      </c>
+      <c r="M17" s="7" t="s">
+        <v>39</v>
+      </c>
+      <c r="N17" s="9"/>
+      <c r="O17" s="9"/>
       <c r="P17" s="2"/>
       <c r="Q17" s="2"/>
       <c r="R17" s="2"/>
@@ -1406,21 +1526,21 @@
       <c r="Z17" s="2"/>
     </row>
     <row r="18">
-      <c r="A18" s="8"/>
-      <c r="B18" s="8"/>
-      <c r="C18" s="8"/>
-      <c r="D18" s="8"/>
-      <c r="E18" s="8"/>
-      <c r="F18" s="8"/>
-      <c r="G18" s="8"/>
-      <c r="H18" s="8"/>
-      <c r="I18" s="8"/>
-      <c r="J18" s="8"/>
-      <c r="K18" s="8"/>
-      <c r="L18" s="8"/>
-      <c r="M18" s="8"/>
-      <c r="N18" s="8"/>
-      <c r="O18" s="8"/>
+      <c r="A18" s="9"/>
+      <c r="B18" s="9"/>
+      <c r="C18" s="9"/>
+      <c r="D18" s="9"/>
+      <c r="E18" s="9"/>
+      <c r="F18" s="9"/>
+      <c r="G18" s="9"/>
+      <c r="H18" s="9"/>
+      <c r="I18" s="9"/>
+      <c r="J18" s="9"/>
+      <c r="K18" s="9"/>
+      <c r="L18" s="9"/>
+      <c r="M18" s="9"/>
+      <c r="N18" s="9"/>
+      <c r="O18" s="9"/>
       <c r="P18" s="2"/>
       <c r="Q18" s="2"/>
       <c r="R18" s="2"/>
@@ -1434,21 +1554,21 @@
       <c r="Z18" s="2"/>
     </row>
     <row r="19">
-      <c r="A19" s="8"/>
-      <c r="B19" s="8"/>
-      <c r="C19" s="8"/>
-      <c r="D19" s="8"/>
-      <c r="E19" s="8"/>
-      <c r="F19" s="8"/>
-      <c r="G19" s="8"/>
-      <c r="H19" s="8"/>
-      <c r="I19" s="8"/>
-      <c r="J19" s="8"/>
-      <c r="K19" s="8"/>
-      <c r="L19" s="8"/>
-      <c r="M19" s="8"/>
-      <c r="N19" s="8"/>
-      <c r="O19" s="8"/>
+      <c r="A19" s="9"/>
+      <c r="B19" s="9"/>
+      <c r="C19" s="9"/>
+      <c r="D19" s="9"/>
+      <c r="E19" s="9"/>
+      <c r="F19" s="9"/>
+      <c r="G19" s="9"/>
+      <c r="H19" s="9"/>
+      <c r="I19" s="9"/>
+      <c r="J19" s="9"/>
+      <c r="K19" s="9"/>
+      <c r="L19" s="9"/>
+      <c r="M19" s="9"/>
+      <c r="N19" s="9"/>
+      <c r="O19" s="9"/>
       <c r="P19" s="2"/>
       <c r="Q19" s="2"/>
       <c r="R19" s="2"/>
@@ -1462,21 +1582,21 @@
       <c r="Z19" s="2"/>
     </row>
     <row r="20">
-      <c r="A20" s="8"/>
-      <c r="B20" s="8"/>
-      <c r="C20" s="8"/>
-      <c r="D20" s="8"/>
-      <c r="E20" s="8"/>
-      <c r="F20" s="8"/>
-      <c r="G20" s="8"/>
-      <c r="H20" s="8"/>
-      <c r="I20" s="8"/>
-      <c r="J20" s="8"/>
-      <c r="K20" s="8"/>
-      <c r="L20" s="8"/>
-      <c r="M20" s="8"/>
-      <c r="N20" s="8"/>
-      <c r="O20" s="8"/>
+      <c r="A20" s="9"/>
+      <c r="B20" s="9"/>
+      <c r="C20" s="9"/>
+      <c r="D20" s="9"/>
+      <c r="E20" s="9"/>
+      <c r="F20" s="9"/>
+      <c r="G20" s="9"/>
+      <c r="H20" s="9"/>
+      <c r="I20" s="9"/>
+      <c r="J20" s="9"/>
+      <c r="K20" s="9"/>
+      <c r="L20" s="9"/>
+      <c r="M20" s="9"/>
+      <c r="N20" s="9"/>
+      <c r="O20" s="9"/>
       <c r="P20" s="2"/>
       <c r="Q20" s="2"/>
       <c r="R20" s="2"/>
@@ -1490,21 +1610,21 @@
       <c r="Z20" s="2"/>
     </row>
     <row r="21" ht="15.75" customHeight="1">
-      <c r="A21" s="8"/>
-      <c r="B21" s="8"/>
-      <c r="C21" s="8"/>
-      <c r="D21" s="8"/>
-      <c r="E21" s="8"/>
-      <c r="F21" s="8"/>
-      <c r="G21" s="8"/>
-      <c r="H21" s="8"/>
-      <c r="I21" s="8"/>
-      <c r="J21" s="8"/>
-      <c r="K21" s="8"/>
-      <c r="L21" s="8"/>
-      <c r="M21" s="8"/>
-      <c r="N21" s="8"/>
-      <c r="O21" s="8"/>
+      <c r="A21" s="9"/>
+      <c r="B21" s="9"/>
+      <c r="C21" s="9"/>
+      <c r="D21" s="9"/>
+      <c r="E21" s="9"/>
+      <c r="F21" s="9"/>
+      <c r="G21" s="9"/>
+      <c r="H21" s="9"/>
+      <c r="I21" s="9"/>
+      <c r="J21" s="9"/>
+      <c r="K21" s="9"/>
+      <c r="L21" s="9"/>
+      <c r="M21" s="9"/>
+      <c r="N21" s="9"/>
+      <c r="O21" s="9"/>
       <c r="P21" s="2"/>
       <c r="Q21" s="2"/>
       <c r="R21" s="2"/>
@@ -1518,21 +1638,21 @@
       <c r="Z21" s="2"/>
     </row>
     <row r="22" ht="15.75" customHeight="1">
-      <c r="A22" s="8"/>
-      <c r="B22" s="8"/>
-      <c r="C22" s="8"/>
-      <c r="D22" s="8"/>
-      <c r="E22" s="8"/>
-      <c r="F22" s="8"/>
-      <c r="G22" s="8"/>
-      <c r="H22" s="8"/>
-      <c r="I22" s="8"/>
-      <c r="J22" s="8"/>
-      <c r="K22" s="8"/>
-      <c r="L22" s="8"/>
-      <c r="M22" s="8"/>
-      <c r="N22" s="8"/>
-      <c r="O22" s="8"/>
+      <c r="A22" s="9"/>
+      <c r="B22" s="9"/>
+      <c r="C22" s="9"/>
+      <c r="D22" s="9"/>
+      <c r="E22" s="9"/>
+      <c r="F22" s="9"/>
+      <c r="G22" s="9"/>
+      <c r="H22" s="9"/>
+      <c r="I22" s="9"/>
+      <c r="J22" s="9"/>
+      <c r="K22" s="9"/>
+      <c r="L22" s="9"/>
+      <c r="M22" s="9"/>
+      <c r="N22" s="9"/>
+      <c r="O22" s="9"/>
       <c r="P22" s="2"/>
       <c r="Q22" s="2"/>
       <c r="R22" s="2"/>
@@ -29042,8 +29162,8 @@
       <c r="Z3" s="2"/>
     </row>
     <row r="4">
-      <c r="A4" s="9" t="s">
-        <v>63</v>
+      <c r="A4" s="10" t="s">
+        <v>82</v>
       </c>
       <c r="B4" s="2"/>
       <c r="C4" s="2"/>
@@ -29072,11 +29192,11 @@
       <c r="Z4" s="2"/>
     </row>
     <row r="5">
-      <c r="A5" s="10" t="s">
-        <v>64</v>
+      <c r="A5" s="11" t="s">
+        <v>83</v>
       </c>
-      <c r="B5" s="10" t="s">
-        <v>65</v>
+      <c r="B5" s="11" t="s">
+        <v>84</v>
       </c>
       <c r="C5" s="2"/>
       <c r="D5" s="2"/>
@@ -29104,12 +29224,12 @@
       <c r="Z5" s="2"/>
     </row>
     <row r="6">
-      <c r="A6" s="11" t="str">
+      <c r="A6" s="12" t="str">
         <f>'Plantilla de Casos de Prueba'!A6</f>
         <v>Id</v>
       </c>
-      <c r="B6" s="11" t="s">
-        <v>66</v>
+      <c r="B6" s="12" t="s">
+        <v>85</v>
       </c>
       <c r="C6" s="2"/>
       <c r="D6" s="2"/>
@@ -29137,12 +29257,12 @@
       <c r="Z6" s="2"/>
     </row>
     <row r="7">
-      <c r="A7" s="11" t="str">
+      <c r="A7" s="12" t="str">
         <f>'Plantilla de Casos de Prueba'!B6</f>
         <v>Caso de Prueba</v>
       </c>
-      <c r="B7" s="11" t="s">
-        <v>67</v>
+      <c r="B7" s="12" t="s">
+        <v>86</v>
       </c>
       <c r="C7" s="2"/>
       <c r="D7" s="2"/>
@@ -29170,12 +29290,12 @@
       <c r="Z7" s="2"/>
     </row>
     <row r="8" ht="30.0" customHeight="1">
-      <c r="A8" s="11" t="str">
+      <c r="A8" s="12" t="str">
         <f>'Plantilla de Casos de Prueba'!C6</f>
         <v>Descripción</v>
       </c>
-      <c r="B8" s="11" t="s">
-        <v>68</v>
+      <c r="B8" s="12" t="s">
+        <v>87</v>
       </c>
       <c r="C8" s="2"/>
       <c r="D8" s="2"/>
@@ -29203,12 +29323,12 @@
       <c r="Z8" s="2"/>
     </row>
     <row r="9">
-      <c r="A9" s="11" t="str">
+      <c r="A9" s="12" t="str">
         <f>'Plantilla de Casos de Prueba'!D6</f>
         <v>Fecha</v>
       </c>
-      <c r="B9" s="11" t="s">
-        <v>69</v>
+      <c r="B9" s="12" t="s">
+        <v>88</v>
       </c>
       <c r="C9" s="2"/>
       <c r="D9" s="2"/>
@@ -29236,12 +29356,12 @@
       <c r="Z9" s="2"/>
     </row>
     <row r="10" ht="45.0" customHeight="1">
-      <c r="A10" s="11" t="str">
+      <c r="A10" s="12" t="str">
         <f>'Plantilla de Casos de Prueba'!E6</f>
         <v>Área Funcional / Sub proceso</v>
       </c>
-      <c r="B10" s="11" t="s">
-        <v>70</v>
+      <c r="B10" s="12" t="s">
+        <v>89</v>
       </c>
       <c r="C10" s="2"/>
       <c r="D10" s="2"/>
@@ -29269,12 +29389,12 @@
       <c r="Z10" s="2"/>
     </row>
     <row r="11" ht="30.0" customHeight="1">
-      <c r="A11" s="11" t="str">
+      <c r="A11" s="12" t="str">
         <f>'Plantilla de Casos de Prueba'!F6</f>
         <v>Funcionalidad / Característica</v>
       </c>
-      <c r="B11" s="11" t="s">
-        <v>71</v>
+      <c r="B11" s="12" t="s">
+        <v>90</v>
       </c>
       <c r="C11" s="2"/>
       <c r="D11" s="2"/>
@@ -29302,12 +29422,12 @@
       <c r="Z11" s="2"/>
     </row>
     <row r="12" ht="45.0" customHeight="1">
-      <c r="A12" s="11" t="str">
+      <c r="A12" s="12" t="str">
         <f>'Plantilla de Casos de Prueba'!G6</f>
         <v>Datos / Acciones de Entrada</v>
       </c>
-      <c r="B12" s="11" t="s">
-        <v>72</v>
+      <c r="B12" s="12" t="s">
+        <v>91</v>
       </c>
       <c r="C12" s="2"/>
       <c r="D12" s="2"/>
@@ -29335,12 +29455,12 @@
       <c r="Z12" s="2"/>
     </row>
     <row r="13">
-      <c r="A13" s="11" t="str">
+      <c r="A13" s="12" t="str">
         <f>'Plantilla de Casos de Prueba'!H6</f>
         <v>Resultado Esperado</v>
       </c>
-      <c r="B13" s="11" t="s">
-        <v>73</v>
+      <c r="B13" s="12" t="s">
+        <v>92</v>
       </c>
       <c r="C13" s="2"/>
       <c r="D13" s="2"/>
@@ -29368,12 +29488,12 @@
       <c r="Z13" s="2"/>
     </row>
     <row r="14" ht="45.0" customHeight="1">
-      <c r="A14" s="11" t="str">
+      <c r="A14" s="12" t="str">
         <f>'Plantilla de Casos de Prueba'!I6</f>
         <v>Requerimientos de Ambiente de Pruebas</v>
       </c>
-      <c r="B14" s="11" t="s">
-        <v>74</v>
+      <c r="B14" s="12" t="s">
+        <v>93</v>
       </c>
       <c r="C14" s="2"/>
       <c r="D14" s="2"/>
@@ -29401,12 +29521,12 @@
       <c r="Z14" s="2"/>
     </row>
     <row r="15" ht="30.0" customHeight="1">
-      <c r="A15" s="11" t="str">
+      <c r="A15" s="12" t="str">
         <f>'Plantilla de Casos de Prueba'!J6</f>
         <v>Procedimientos especiales requeridos</v>
       </c>
-      <c r="B15" s="11" t="s">
-        <v>75</v>
+      <c r="B15" s="12" t="s">
+        <v>94</v>
       </c>
       <c r="C15" s="2"/>
       <c r="D15" s="2"/>
@@ -29434,12 +29554,12 @@
       <c r="Z15" s="2"/>
     </row>
     <row r="16" ht="30.0" customHeight="1">
-      <c r="A16" s="11" t="str">
+      <c r="A16" s="12" t="str">
         <f>'Plantilla de Casos de Prueba'!K6</f>
         <v>Dependencias con otros casos de Prueba</v>
       </c>
-      <c r="B16" s="11" t="s">
-        <v>76</v>
+      <c r="B16" s="12" t="s">
+        <v>95</v>
       </c>
       <c r="C16" s="2"/>
       <c r="D16" s="2"/>
@@ -29467,10 +29587,10 @@
       <c r="Z16" s="2"/>
     </row>
     <row r="17">
-      <c r="A17" s="12" t="s">
-        <v>77</v>
+      <c r="A17" s="13" t="s">
+        <v>96</v>
       </c>
-      <c r="B17" s="13"/>
+      <c r="B17" s="14"/>
       <c r="C17" s="2"/>
       <c r="D17" s="2"/>
       <c r="E17" s="2"/>
@@ -29497,12 +29617,12 @@
       <c r="Z17" s="2"/>
     </row>
     <row r="18" ht="30.0" customHeight="1">
-      <c r="A18" s="11" t="str">
+      <c r="A18" s="12" t="str">
         <f>'Plantilla de Casos de Prueba'!L6</f>
         <v>Resultado Obtenido</v>
       </c>
-      <c r="B18" s="11" t="s">
-        <v>78</v>
+      <c r="B18" s="12" t="s">
+        <v>97</v>
       </c>
       <c r="C18" s="2"/>
       <c r="D18" s="2"/>
@@ -29530,12 +29650,12 @@
       <c r="Z18" s="2"/>
     </row>
     <row r="19">
-      <c r="A19" s="11" t="str">
+      <c r="A19" s="12" t="str">
         <f>'Plantilla de Casos de Prueba'!M6</f>
         <v>Estado</v>
       </c>
-      <c r="B19" s="11" t="s">
-        <v>79</v>
+      <c r="B19" s="12" t="s">
+        <v>98</v>
       </c>
       <c r="C19" s="2"/>
       <c r="D19" s="2"/>
@@ -29563,12 +29683,12 @@
       <c r="Z19" s="2"/>
     </row>
     <row r="20">
-      <c r="A20" s="11" t="str">
+      <c r="A20" s="12" t="str">
         <f>'Plantilla de Casos de Prueba'!N6</f>
         <v>Última Fecha de Estado</v>
       </c>
-      <c r="B20" s="11" t="s">
-        <v>80</v>
+      <c r="B20" s="12" t="s">
+        <v>99</v>
       </c>
       <c r="C20" s="2"/>
       <c r="D20" s="2"/>
@@ -29596,12 +29716,12 @@
       <c r="Z20" s="2"/>
     </row>
     <row r="21" ht="15.75" customHeight="1">
-      <c r="A21" s="11" t="str">
+      <c r="A21" s="12" t="str">
         <f>'Plantilla de Casos de Prueba'!O6</f>
         <v>Observaciones</v>
       </c>
-      <c r="B21" s="11" t="s">
-        <v>81</v>
+      <c r="B21" s="12" t="s">
+        <v>100</v>
       </c>
       <c r="C21" s="2"/>
       <c r="D21" s="2"/>

</xml_diff>